<commit_message>
Update Grupos De Utilizadores
Alteração nas funcionalidades da direção.
</commit_message>
<xml_diff>
--- a/Grupos De Utilizadores.xlsx
+++ b/Grupos De Utilizadores.xlsx
@@ -103,9 +103,6 @@
     <t>Edição de perfil pessoal; Remover Utilizador; Adicionar Utilizador; Editar Utilizador; Redação de notificações;</t>
   </si>
   <si>
-    <t>Consulta de perfis; Consulta de notificações; Consulta estatísticas de turma; Consultar estatísticas da escola;</t>
-  </si>
-  <si>
     <t>Resolução de exercícios/fichas propostos; Consulta de exercícios/fichas já realizados(as) e respetivas notas.</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Diretor</t>
+  </si>
+  <si>
+    <t>Consulta de perfis; Consulta de notificações; Consulta de estatísticas de aluno; Consulta estatísticas de turma; Consultar estatísticas da escola;</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -291,36 +291,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -364,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -372,15 +350,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,38 +358,41 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,34 +700,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="1.140625" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="120" customWidth="1"/>
+    <col min="5" max="5" width="125.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -766,7 +738,7 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -777,7 +749,7 @@
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -788,29 +760,29 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -819,13 +791,13 @@
     </row>
     <row r="10" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -833,7 +805,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -841,7 +813,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -849,33 +821,33 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="14"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="22"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
@@ -884,13 +856,13 @@
     </row>
     <row r="20" spans="4:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -898,15 +870,15 @@
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -914,33 +886,33 @@
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="18"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="22"/>
-      <c r="E26" s="24"/>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -949,21 +921,21 @@
     </row>
     <row r="30" spans="4:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="6" t="s">
@@ -971,7 +943,7 @@
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -979,33 +951,33 @@
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="16"/>
-      <c r="E36" s="18"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="20"/>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="6" t="s">
@@ -1014,6 +986,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="E15:E16"/>
@@ -1023,11 +1000,6 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>